<commit_message>
Update docs with new stuff
</commit_message>
<xml_diff>
--- a/Charges.xlsx
+++ b/Charges.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Documents\Code Gate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CRI\Poratil CPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Charges Description</t>
   </si>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>42667</v>
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="C5" s="3">
         <v>42668</v>
@@ -507,13 +507,24 @@
         <v>42668</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42669</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1">
         <f>SUM(B4:B21)</f>
-        <v>50075</v>
+        <v>50113.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>